<commit_message>
1.0 code and Results
Cleaned up 1.0 code and finished up results for the four test files
(only one actually finished)
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="6360" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="3700" yWindow="6540" windowWidth="34100" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -27,32 +27,44 @@
     <t>Description of Implementation/Changes</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Results: youtube.txt: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nodes: 1134890 Edges: 2987624</t>
-    </r>
-  </si>
-  <si>
     <t>Too long to measure</t>
   </si>
   <si>
-    <t>Results: amazon.txt: Nodes: 334863 Edges: 925872</t>
+    <t>5.82824s</t>
+  </si>
+  <si>
+    <t>youtube.txt</t>
+  </si>
+  <si>
+    <t>amazon.txt</t>
+  </si>
+  <si>
+    <t>enron.txt</t>
+  </si>
+  <si>
+    <t>cagrqc.txt</t>
+  </si>
+  <si>
+    <t>Nodes: 5242 Edges: 28980 Triangles: 48260</t>
+  </si>
+  <si>
+    <t>Nodes: 36692 Edges: 367662 Triangles: 727044</t>
+  </si>
+  <si>
+    <t>Nodes: 334863 Edges: 925872 Triangles: 667129</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nodes: 1134890 Edges: 2987624 Triangles: 3056386</t>
+  </si>
+  <si>
+    <t>Two vectors of pairs of int's, three pairs of ints stored into a struct</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -61,8 +73,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -85,14 +106,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,46 +462,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>41911</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>41911</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>